<commit_message>
update excel, update several classes, add of the possibility of modification
</commit_message>
<xml_diff>
--- a/Gestion projet S2.xlsx
+++ b/Gestion projet S2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="72" windowWidth="18912" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="1140" windowWidth="12792" windowHeight="6576"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -417,7 +418,7 @@
           <c:x val="7.4261381217349431E-2"/>
           <c:y val="7.3740535479704702E-2"/>
           <c:w val="0.78083130537451662"/>
-          <c:h val="0.83089630762737055"/>
+          <c:h val="0.83089630762737066"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -480,6 +481,9 @@
                 <c:pt idx="12">
                   <c:v>7390</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>7325</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -565,25 +569,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="127034112"/>
-        <c:axId val="127035648"/>
+        <c:axId val="95703808"/>
+        <c:axId val="95705344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127034112"/>
+        <c:axId val="95703808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127035648"/>
+        <c:crossAx val="95705344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127035648"/>
+        <c:axId val="95705344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +614,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127034112"/>
+        <c:crossAx val="95703808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -624,7 +628,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -952,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2073,45 +2077,62 @@
       <c r="F16" s="11">
         <v>12</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="G16" s="11">
+        <v>2</v>
+      </c>
+      <c r="H16" s="11">
+        <v>2</v>
+      </c>
+      <c r="I16" s="11">
+        <v>2</v>
+      </c>
       <c r="J16" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="K16" s="11">
+        <v>2</v>
+      </c>
+      <c r="L16" s="11">
+        <v>1</v>
+      </c>
+      <c r="M16" s="11">
+        <v>1</v>
+      </c>
       <c r="N16" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O16" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P16" s="11">
         <v>15</v>
       </c>
-      <c r="Q16" s="11"/>
+      <c r="Q16" s="11">
+        <v>15</v>
+      </c>
       <c r="R16" s="11">
         <v>100</v>
       </c>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11">
-        <v>100</v>
-      </c>
+      <c r="S16" s="11">
+        <v>100</v>
+      </c>
+      <c r="T16" s="11"/>
       <c r="U16" s="11"/>
       <c r="V16" s="11">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>380</v>
       </c>
       <c r="W16" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X16" s="11"/>
+        <v>315</v>
+      </c>
+      <c r="X16" s="11">
+        <f>SUM($W$3:W16)+SUM(V17:$V$23)</f>
+        <v>7325</v>
+      </c>
       <c r="Y16" s="11">
         <v>8675</v>
       </c>
@@ -2217,11 +2238,13 @@
         <v>100</v>
       </c>
       <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
+      <c r="T18" s="11">
+        <v>100</v>
+      </c>
       <c r="U18" s="11"/>
       <c r="V18" s="11">
         <f t="shared" si="2"/>
-        <v>380</v>
+        <v>480</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="3"/>
@@ -2510,7 +2533,7 @@
       </c>
       <c r="W24" s="5">
         <f>SUM(W4,W3,W5,W6,W7,W8,W9,W10,W11,W12,W13,W14,W15,W17,W16,W18,W19,W20,W21,W22,W23)</f>
-        <v>3730</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -2520,15 +2543,15 @@
       </c>
       <c r="G25">
         <f>SUM(G3:G22)+SUM(K3:K22)</f>
-        <v>44.5</v>
+        <v>48.5</v>
       </c>
       <c r="H25">
         <f>SUM(H3:H22)+SUM(L3:L22)</f>
-        <v>37.5</v>
+        <v>40.5</v>
       </c>
       <c r="I25">
         <f>SUM(I3:I22)+SUM(M3:M22)</f>
-        <v>40.5</v>
+        <v>43.5</v>
       </c>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>

</xml_diff>

<commit_message>
update excel gestion projet. Add first ihms
</commit_message>
<xml_diff>
--- a/Gestion projet S2.xlsx
+++ b/Gestion projet S2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="16080" windowHeight="9975"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13545" windowHeight="8640"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -593,11 +594,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="178600960"/>
-        <c:axId val="178627328"/>
+        <c:axId val="160146560"/>
+        <c:axId val="160148096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="178600960"/>
+        <c:axId val="160146560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +607,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178627328"/>
+        <c:crossAx val="160148096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,7 +615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178627328"/>
+        <c:axId val="160148096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +645,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178600960"/>
+        <c:crossAx val="160146560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -991,7 +992,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,29 +2191,35 @@
       <c r="F17" s="11">
         <v>12</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="G17" s="11">
+        <v>2</v>
+      </c>
+      <c r="H17" s="11">
+        <v>2</v>
+      </c>
+      <c r="I17" s="11">
+        <v>2</v>
+      </c>
       <c r="J17" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K17" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L17" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M17" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N17" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O17" s="11">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="P17" s="11">
         <v>15</v>
@@ -2230,7 +2237,7 @@
       </c>
       <c r="W17" s="11">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>320</v>
       </c>
       <c r="X17" s="11"/>
       <c r="Y17" s="11">
@@ -2575,7 +2582,7 @@
       </c>
       <c r="W24" s="5">
         <f>SUM(W4,W3,W5,W6,W7,W8,W9,W10,W11,W12,W13,W14,W15,W17,W16,W18,W19,W20,W21,W22,W23)</f>
-        <v>4205</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -2585,15 +2592,15 @@
       </c>
       <c r="G25">
         <f>SUM(G3:G22)+SUM(K3:K22)</f>
-        <v>48.5</v>
+        <v>53.5</v>
       </c>
       <c r="H25">
         <f>SUM(H3:H22)+SUM(L3:L22)</f>
-        <v>42.5</v>
+        <v>45.5</v>
       </c>
       <c r="I25">
         <f>SUM(I3:I22)+SUM(M3:M22)</f>
-        <v>49.5</v>
+        <v>52.5</v>
       </c>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>

</xml_diff>

<commit_message>
update color black to grey update GUI F11 key for fullscreen update Gestion projet
</commit_message>
<xml_diff>
--- a/Gestion projet S2.xlsx
+++ b/Gestion projet S2.xlsx
@@ -480,25 +480,28 @@
                   <c:v>8270</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8170</c:v>
+                  <c:v>8270</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8205</c:v>
+                  <c:v>8305</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7900</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7595</c:v>
+                  <c:v>7695</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7450</c:v>
+                  <c:v>7550</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7385</c:v>
+                  <c:v>7485</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7540</c:v>
+                  <c:v>7520</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7815</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -596,11 +599,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="186657408"/>
-        <c:axId val="186847616"/>
+        <c:axId val="180028928"/>
+        <c:axId val="180030464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="186657408"/>
+        <c:axId val="180028928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +612,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186847616"/>
+        <c:crossAx val="180030464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -617,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186847616"/>
+        <c:axId val="180030464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +650,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186657408"/>
+        <c:crossAx val="180028928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -994,7 +997,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,7 +1475,9 @@
       <c r="R7" s="11">
         <v>100</v>
       </c>
-      <c r="S7" s="11"/>
+      <c r="S7" s="11">
+        <v>0</v>
+      </c>
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
       <c r="V7" s="11">
@@ -1786,18 +1791,20 @@
       <c r="T11" s="11">
         <v>100</v>
       </c>
-      <c r="U11" s="11"/>
+      <c r="U11" s="11">
+        <v>100</v>
+      </c>
       <c r="V11" s="11">
         <f t="shared" si="2"/>
         <v>475</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="3"/>
-        <v>375</v>
+        <v>475</v>
       </c>
       <c r="X11" s="11">
         <f>SUM($W$3:W11)+SUM(V12:$V$23)</f>
-        <v>8170</v>
+        <v>8270</v>
       </c>
       <c r="Y11" s="11">
         <v>8675</v>
@@ -1876,7 +1883,7 @@
       </c>
       <c r="X12" s="11">
         <f>SUM($W$3:W12)+SUM(V13:$V$23)</f>
-        <v>8205</v>
+        <v>8305</v>
       </c>
       <c r="Y12" s="11">
         <v>8675</v>
@@ -1947,7 +1954,7 @@
       </c>
       <c r="X13" s="11">
         <f>SUM($W$3:W13)+SUM(V14:$V$23)</f>
-        <v>7900</v>
+        <v>8000</v>
       </c>
       <c r="Y13" s="11">
         <v>8675</v>
@@ -2020,7 +2027,7 @@
       </c>
       <c r="X14" s="11">
         <f>SUM($W$3:W14)+SUM(V15:$V$23)</f>
-        <v>7595</v>
+        <v>7695</v>
       </c>
       <c r="Y14" s="11">
         <v>8675</v>
@@ -2093,7 +2100,7 @@
       </c>
       <c r="X15" s="11">
         <f>SUM($W$3:W15)+SUM(V16:$V$23)</f>
-        <v>7450</v>
+        <v>7550</v>
       </c>
       <c r="Y15" s="11">
         <v>8675</v>
@@ -2170,7 +2177,7 @@
       </c>
       <c r="X16" s="11">
         <f>SUM($W$3:W16)+SUM(V17:$V$23)</f>
-        <v>7385</v>
+        <v>7485</v>
       </c>
       <c r="Y16" s="11">
         <v>8675</v>
@@ -2207,21 +2214,21 @@
         <v>3</v>
       </c>
       <c r="K17" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L17" s="11">
         <v>4</v>
       </c>
       <c r="M17" s="11">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N17" s="11">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="O17" s="11">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P17" s="11">
         <v>15</v>
@@ -2243,11 +2250,11 @@
       </c>
       <c r="W17" s="11">
         <f t="shared" si="3"/>
-        <v>535</v>
+        <v>415</v>
       </c>
       <c r="X17" s="11">
         <f>SUM($W$3:W17)+SUM(V18:$V$23)</f>
-        <v>7540</v>
+        <v>7520</v>
       </c>
       <c r="Y17" s="11">
         <v>8675</v>
@@ -2270,45 +2277,62 @@
       <c r="F18" s="11">
         <v>12</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18" s="11">
+        <v>1</v>
+      </c>
+      <c r="I18" s="11">
+        <v>1</v>
+      </c>
       <c r="J18" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="K18" s="11">
+        <v>9</v>
+      </c>
+      <c r="L18" s="11">
+        <v>5</v>
+      </c>
+      <c r="M18" s="11">
+        <v>11</v>
+      </c>
       <c r="N18" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="O18" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P18" s="11">
         <v>15</v>
       </c>
-      <c r="Q18" s="11"/>
+      <c r="Q18" s="11">
+        <v>15</v>
+      </c>
       <c r="R18" s="11">
         <v>100</v>
       </c>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11">
-        <v>100</v>
-      </c>
+      <c r="S18" s="11">
+        <v>100</v>
+      </c>
+      <c r="T18" s="11"/>
       <c r="U18" s="11"/>
       <c r="V18" s="11">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>380</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X18" s="11"/>
+        <v>675</v>
+      </c>
+      <c r="X18" s="11">
+        <f>SUM($W$3:W18)+SUM(V19:$V$23)</f>
+        <v>7815</v>
+      </c>
       <c r="Y18" s="11">
         <v>8675</v>
       </c>
@@ -2339,16 +2363,22 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="K19" s="11">
+        <v>1</v>
+      </c>
+      <c r="L19" s="11">
+        <v>1</v>
+      </c>
+      <c r="M19" s="11">
+        <v>1</v>
+      </c>
       <c r="N19" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O19" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P19" s="11">
         <v>15</v>
@@ -2358,15 +2388,17 @@
         <v>100</v>
       </c>
       <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
+      <c r="T19" s="11">
+        <v>100</v>
+      </c>
       <c r="U19" s="11"/>
       <c r="V19" s="11">
         <f t="shared" si="2"/>
-        <v>380</v>
+        <v>480</v>
       </c>
       <c r="W19" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="X19" s="11"/>
       <c r="Y19" s="11">
@@ -2591,7 +2623,7 @@
       </c>
       <c r="W24" s="5">
         <f>SUM(W4,W3,W5,W6,W7,W8,W9,W10,W11,W12,W13,W14,W15,W17,W16,W18,W19,W20,W21,W22,W23)</f>
-        <v>4640</v>
+        <v>5355</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -2601,15 +2633,15 @@
       </c>
       <c r="G25">
         <f>SUM(G3:G22)+SUM(K3:K22)</f>
-        <v>54.5</v>
+        <v>64.5</v>
       </c>
       <c r="H25">
         <f>SUM(H3:H22)+SUM(L3:L22)</f>
-        <v>45.5</v>
+        <v>52.5</v>
       </c>
       <c r="I25">
         <f>SUM(I3:I22)+SUM(M3:M22)</f>
-        <v>56.5</v>
+        <v>64.5</v>
       </c>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>

</xml_diff>

<commit_message>
added limit ship zone. Improved ship path.
</commit_message>
<xml_diff>
--- a/Gestion projet S2.xlsx
+++ b/Gestion projet S2.xlsx
@@ -178,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -333,14 +333,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -361,13 +371,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,6 +515,9 @@
                 <c:pt idx="15">
                   <c:v>7815</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>8030</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -599,11 +614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="180028928"/>
-        <c:axId val="180030464"/>
+        <c:axId val="185612160"/>
+        <c:axId val="185613696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180028928"/>
+        <c:axId val="185612160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +627,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180030464"/>
+        <c:crossAx val="185613696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180030464"/>
+        <c:axId val="185613696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,7 +665,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180028928"/>
+        <c:crossAx val="185612160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -996,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,1645 +1044,1652 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="7" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="Q1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="X1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="24" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="13"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="12"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>42401</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11">
-        <v>12</v>
-      </c>
-      <c r="E3" s="11">
-        <v>0</v>
-      </c>
-      <c r="F3" s="11">
-        <v>12</v>
-      </c>
-      <c r="G3" s="11">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>12</v>
+      </c>
+      <c r="G3" s="10">
         <v>2.5</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>2.5</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="10">
         <v>2.5</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <f>G3+H3+I3</f>
         <v>7.5</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10">
         <f>K3+M3+L3</f>
         <v>0</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="10">
         <f>J3+N3</f>
         <v>7.5</v>
       </c>
-      <c r="P3" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="11">
-        <v>15</v>
-      </c>
-      <c r="R3" s="11">
-        <v>100</v>
-      </c>
-      <c r="S3" s="11">
-        <v>100</v>
-      </c>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11">
+      <c r="P3" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>15</v>
+      </c>
+      <c r="R3" s="10">
+        <v>100</v>
+      </c>
+      <c r="S3" s="10">
+        <v>100</v>
+      </c>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10">
         <f>20*D3+22.5*E3+P3+T3+R3</f>
         <v>355</v>
       </c>
-      <c r="W3" s="11">
+      <c r="W3" s="10">
         <f>J3*20+N3*20+Q3+U3+S3</f>
         <v>265</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="10">
         <f>SUM(W3,V4:V23)</f>
         <v>8575</v>
       </c>
-      <c r="Y3" s="11">
+      <c r="Y3" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>42408</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11">
-        <v>12</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0</v>
-      </c>
-      <c r="F4" s="11">
-        <v>12</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10">
+        <v>12</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>12</v>
+      </c>
+      <c r="G4" s="10">
         <v>2.5</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>2.5</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>2.5</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <f>G4+H4+I4</f>
         <v>7.5</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11">
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10">
         <f t="shared" ref="N4:N22" si="0">K4+M4+L4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="10">
         <f t="shared" ref="O4:O22" si="1">J4+N4</f>
         <v>7.5</v>
       </c>
-      <c r="P4" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="11">
-        <v>15</v>
-      </c>
-      <c r="R4" s="11">
-        <v>100</v>
-      </c>
-      <c r="S4" s="11">
-        <v>100</v>
-      </c>
-      <c r="T4" s="11">
-        <v>100</v>
-      </c>
-      <c r="U4" s="11">
-        <v>100</v>
-      </c>
-      <c r="V4" s="11">
+      <c r="P4" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>15</v>
+      </c>
+      <c r="R4" s="10">
+        <v>100</v>
+      </c>
+      <c r="S4" s="10">
+        <v>100</v>
+      </c>
+      <c r="T4" s="10">
+        <v>100</v>
+      </c>
+      <c r="U4" s="10">
+        <v>100</v>
+      </c>
+      <c r="V4" s="10">
         <f t="shared" ref="V4:V22" si="2">20*D4+22.5*E4+P4+T4+R4</f>
         <v>455</v>
       </c>
-      <c r="W4" s="11">
+      <c r="W4" s="10">
         <f t="shared" ref="W4:W22" si="3">J4*20+N4*20+Q4+U4+S4</f>
         <v>365</v>
       </c>
-      <c r="X4" s="11">
+      <c r="X4" s="10">
         <f>SUM(W3,W4,V5:V23)</f>
         <v>8485</v>
       </c>
-      <c r="Y4" s="11">
+      <c r="Y4" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>42415</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11">
-        <v>12</v>
-      </c>
-      <c r="E5" s="11">
-        <v>0</v>
-      </c>
-      <c r="F5" s="11">
-        <v>12</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="D5" s="10">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>12</v>
+      </c>
+      <c r="G5" s="10">
         <v>4</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>4</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>4</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <f>G5+H5+I5</f>
         <v>12</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11">
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="P5" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="11">
-        <v>15</v>
-      </c>
-      <c r="R5" s="11">
-        <v>100</v>
-      </c>
-      <c r="S5" s="11">
-        <v>100</v>
-      </c>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11">
+      <c r="P5" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>15</v>
+      </c>
+      <c r="R5" s="10">
+        <v>100</v>
+      </c>
+      <c r="S5" s="10">
+        <v>100</v>
+      </c>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10">
         <f t="shared" si="2"/>
         <v>355</v>
       </c>
-      <c r="W5" s="11">
+      <c r="W5" s="10">
         <f t="shared" si="3"/>
         <v>355</v>
       </c>
-      <c r="X5" s="11">
+      <c r="X5" s="10">
         <f>SUM(W3:W5,V6:V23)</f>
         <v>8485</v>
       </c>
-      <c r="Y5" s="11">
+      <c r="Y5" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>42422</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10">
         <v>8</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>4</v>
       </c>
-      <c r="F6" s="11">
-        <v>12</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="F6" s="10">
+        <v>12</v>
+      </c>
+      <c r="G6" s="10">
         <v>4.5</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>4.5</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>4.5</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f t="shared" ref="J6:J22" si="4">G6+H6+I6</f>
         <v>13.5</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11">
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="10">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="P6" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>15</v>
-      </c>
-      <c r="R6" s="11">
-        <v>100</v>
-      </c>
-      <c r="S6" s="11">
-        <v>100</v>
-      </c>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11">
+      <c r="P6" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>15</v>
+      </c>
+      <c r="R6" s="10">
+        <v>100</v>
+      </c>
+      <c r="S6" s="10">
+        <v>100</v>
+      </c>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10">
         <f t="shared" si="2"/>
         <v>365</v>
       </c>
-      <c r="W6" s="11">
+      <c r="W6" s="10">
         <f t="shared" si="3"/>
         <v>385</v>
       </c>
-      <c r="X6" s="11">
+      <c r="X6" s="10">
         <f>SUM(W3:W6,V7:V23)</f>
         <v>8505</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Y6" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>42429</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10">
         <v>8</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>4</v>
       </c>
-      <c r="F7" s="11">
-        <v>12</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11">
-        <v>0</v>
-      </c>
-      <c r="I7" s="11">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11">
+      <c r="F7" s="10">
+        <v>12</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11">
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P7" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11">
-        <v>100</v>
-      </c>
-      <c r="S7" s="11">
-        <v>0</v>
-      </c>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11">
+      <c r="P7" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10">
+        <v>100</v>
+      </c>
+      <c r="S7" s="10">
+        <v>0</v>
+      </c>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10">
         <f t="shared" si="2"/>
         <v>365</v>
       </c>
-      <c r="W7" s="11">
+      <c r="W7" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X7" s="11">
+      <c r="X7" s="10">
         <f>SUM(W3:W7)+SUM(V8:V23)</f>
         <v>8140</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="Y7" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>42436</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>6</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>6</v>
       </c>
-      <c r="F8" s="11">
-        <v>12</v>
-      </c>
-      <c r="G8" s="11">
+      <c r="F8" s="10">
+        <v>12</v>
+      </c>
+      <c r="G8" s="10">
         <v>4</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>4</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>4</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <v>3</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <v>1</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="10">
         <v>1</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="P8" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="11">
-        <v>15</v>
-      </c>
-      <c r="R8" s="11">
-        <v>100</v>
-      </c>
-      <c r="S8" s="11">
-        <v>100</v>
-      </c>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11">
+      <c r="P8" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>15</v>
+      </c>
+      <c r="R8" s="10">
+        <v>100</v>
+      </c>
+      <c r="S8" s="10">
+        <v>100</v>
+      </c>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10">
         <f t="shared" si="2"/>
         <v>370</v>
       </c>
-      <c r="W8" s="11">
+      <c r="W8" s="10">
         <f t="shared" si="3"/>
         <v>455</v>
       </c>
-      <c r="X8" s="11">
+      <c r="X8" s="10">
         <f>SUM(W3:W8)+SUM(V9:V23)</f>
         <v>8225</v>
       </c>
-      <c r="Y8" s="11">
+      <c r="Y8" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>42443</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10">
         <v>6</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>6</v>
       </c>
-      <c r="F9" s="11">
-        <v>12</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="F9" s="10">
+        <v>12</v>
+      </c>
+      <c r="G9" s="10">
         <v>4</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>4</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>4</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>1</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>0.5</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <v>0.5</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="P9" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="11">
-        <v>15</v>
-      </c>
-      <c r="R9" s="11">
-        <v>100</v>
-      </c>
-      <c r="S9" s="11">
-        <v>100</v>
-      </c>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11">
+      <c r="P9" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>15</v>
+      </c>
+      <c r="R9" s="10">
+        <v>100</v>
+      </c>
+      <c r="S9" s="10">
+        <v>100</v>
+      </c>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10">
         <f t="shared" si="2"/>
         <v>370</v>
       </c>
-      <c r="W9" s="11">
+      <c r="W9" s="10">
         <f t="shared" si="3"/>
         <v>395</v>
       </c>
-      <c r="X9" s="11">
+      <c r="X9" s="10">
         <f>SUM($W$3:$W$9)+SUM($V$10:$V$23)</f>
         <v>8250</v>
       </c>
-      <c r="Y9" s="11">
+      <c r="Y9" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>42450</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10">
         <v>4</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>8</v>
       </c>
-      <c r="F10" s="11">
-        <v>12</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="F10" s="10">
+        <v>12</v>
+      </c>
+      <c r="G10" s="10">
         <v>3</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>3</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>3</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <v>3</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <v>1</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="10">
         <v>1</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="P10" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q10" s="11">
-        <v>15</v>
-      </c>
-      <c r="R10" s="11">
-        <v>100</v>
-      </c>
-      <c r="S10" s="11">
-        <v>100</v>
-      </c>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11">
+      <c r="P10" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>15</v>
+      </c>
+      <c r="R10" s="10">
+        <v>100</v>
+      </c>
+      <c r="S10" s="10">
+        <v>100</v>
+      </c>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10">
         <f t="shared" si="2"/>
         <v>375</v>
       </c>
-      <c r="W10" s="11">
+      <c r="W10" s="10">
         <f t="shared" si="3"/>
         <v>395</v>
       </c>
-      <c r="X10" s="11">
+      <c r="X10" s="10">
         <f>SUM($W$3:W10)+SUM(V11:$V$23)</f>
         <v>8270</v>
       </c>
-      <c r="Y10" s="11">
+      <c r="Y10" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>42457</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10">
         <v>4</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>8</v>
       </c>
-      <c r="F11" s="11">
-        <v>12</v>
-      </c>
-      <c r="G11" s="11">
+      <c r="F11" s="10">
+        <v>12</v>
+      </c>
+      <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>1</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>1</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>4</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>2.5</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <v>3.5</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="P11" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q11" s="11">
-        <v>15</v>
-      </c>
-      <c r="R11" s="11">
-        <v>100</v>
-      </c>
-      <c r="S11" s="11">
-        <v>100</v>
-      </c>
-      <c r="T11" s="11">
-        <v>100</v>
-      </c>
-      <c r="U11" s="11">
-        <v>100</v>
-      </c>
-      <c r="V11" s="11">
+      <c r="P11" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>15</v>
+      </c>
+      <c r="R11" s="10">
+        <v>100</v>
+      </c>
+      <c r="S11" s="10">
+        <v>100</v>
+      </c>
+      <c r="T11" s="10">
+        <v>100</v>
+      </c>
+      <c r="U11" s="10">
+        <v>100</v>
+      </c>
+      <c r="V11" s="10">
         <f t="shared" si="2"/>
         <v>475</v>
       </c>
-      <c r="W11" s="11">
+      <c r="W11" s="10">
         <f t="shared" si="3"/>
         <v>475</v>
       </c>
-      <c r="X11" s="11">
+      <c r="X11" s="10">
         <f>SUM($W$3:W11)+SUM(V12:$V$23)</f>
         <v>8270</v>
       </c>
-      <c r="Y11" s="11">
+      <c r="Y11" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>42464</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>2</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>10</v>
       </c>
-      <c r="F12" s="11">
-        <v>12</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="F12" s="10">
+        <v>12</v>
+      </c>
+      <c r="G12" s="10">
         <v>1</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>1</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>1</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="10">
         <v>4</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <v>4</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="10">
         <v>4</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="P12" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q12" s="11">
-        <v>15</v>
-      </c>
-      <c r="R12" s="11">
-        <v>100</v>
-      </c>
-      <c r="S12" s="11">
-        <v>100</v>
-      </c>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11">
+      <c r="P12" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>15</v>
+      </c>
+      <c r="R12" s="10">
+        <v>100</v>
+      </c>
+      <c r="S12" s="10">
+        <v>100</v>
+      </c>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W12" s="11">
+      <c r="W12" s="10">
         <f t="shared" si="3"/>
         <v>415</v>
       </c>
-      <c r="X12" s="11">
+      <c r="X12" s="10">
         <f>SUM($W$3:W12)+SUM(V13:$V$23)</f>
         <v>8305</v>
       </c>
-      <c r="Y12" s="11">
+      <c r="Y12" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>42471</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10">
         <v>2</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>10</v>
       </c>
-      <c r="F13" s="11">
-        <v>12</v>
-      </c>
-      <c r="G13" s="11">
+      <c r="F13" s="10">
+        <v>12</v>
+      </c>
+      <c r="G13" s="10">
         <v>1</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>1</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>1</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11">
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="10">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="P13" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q13" s="11">
-        <v>15</v>
-      </c>
-      <c r="R13" s="11">
-        <v>100</v>
-      </c>
-      <c r="S13" s="11">
-        <v>0</v>
-      </c>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11">
+      <c r="P13" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>15</v>
+      </c>
+      <c r="R13" s="10">
+        <v>100</v>
+      </c>
+      <c r="S13" s="10">
+        <v>0</v>
+      </c>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W13" s="11">
+      <c r="W13" s="10">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="X13" s="11">
+      <c r="X13" s="10">
         <f>SUM($W$3:W13)+SUM(V14:$V$23)</f>
         <v>8000</v>
       </c>
-      <c r="Y13" s="11">
+      <c r="Y13" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>12</v>
-      </c>
-      <c r="B14" s="12">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11">
         <v>42478</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10">
         <v>2</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>10</v>
       </c>
-      <c r="F14" s="11">
-        <v>12</v>
-      </c>
-      <c r="G14" s="11">
-        <v>0</v>
-      </c>
-      <c r="H14" s="11">
-        <v>0</v>
-      </c>
-      <c r="I14" s="11">
-        <v>0</v>
-      </c>
-      <c r="J14" s="11">
+      <c r="F14" s="10">
+        <v>12</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11">
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10">
         <v>3</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O14" s="10">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="P14" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q14" s="11">
-        <v>15</v>
-      </c>
-      <c r="R14" s="11">
-        <v>100</v>
-      </c>
-      <c r="S14" s="11">
-        <v>0</v>
-      </c>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11">
+      <c r="P14" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>15</v>
+      </c>
+      <c r="R14" s="10">
+        <v>100</v>
+      </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W14" s="11">
+      <c r="W14" s="10">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="X14" s="11">
+      <c r="X14" s="10">
         <f>SUM($W$3:W14)+SUM(V15:$V$23)</f>
         <v>7695</v>
       </c>
-      <c r="Y14" s="11">
+      <c r="Y14" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>42485</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10">
         <v>2</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>10</v>
       </c>
-      <c r="F15" s="11">
-        <v>12</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="F15" s="10">
+        <v>12</v>
+      </c>
+      <c r="G15" s="10">
         <v>2</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>1</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <v>1</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="10">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11">
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10">
         <v>2</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="P15" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>15</v>
-      </c>
-      <c r="R15" s="11">
-        <v>100</v>
-      </c>
-      <c r="S15" s="11">
-        <v>100</v>
-      </c>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11">
+      <c r="P15" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>15</v>
+      </c>
+      <c r="R15" s="10">
+        <v>100</v>
+      </c>
+      <c r="S15" s="10">
+        <v>100</v>
+      </c>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W15" s="11">
+      <c r="W15" s="10">
         <f t="shared" si="3"/>
         <v>235</v>
       </c>
-      <c r="X15" s="11">
+      <c r="X15" s="10">
         <f>SUM($W$3:W15)+SUM(V16:$V$23)</f>
         <v>7550</v>
       </c>
-      <c r="Y15" s="11">
+      <c r="Y15" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>42492</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10">
         <v>2</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>10</v>
       </c>
-      <c r="F16" s="11">
-        <v>12</v>
-      </c>
-      <c r="G16" s="11">
+      <c r="F16" s="10">
+        <v>12</v>
+      </c>
+      <c r="G16" s="10">
         <v>2</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>2</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>2</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="10">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="10">
         <v>2</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <v>1</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="10">
         <v>1</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="10">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="P16" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q16" s="11">
-        <v>15</v>
-      </c>
-      <c r="R16" s="11">
-        <v>100</v>
-      </c>
-      <c r="S16" s="11">
-        <v>100</v>
-      </c>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11">
+      <c r="P16" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>15</v>
+      </c>
+      <c r="R16" s="10">
+        <v>100</v>
+      </c>
+      <c r="S16" s="10">
+        <v>100</v>
+      </c>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W16" s="11">
+      <c r="W16" s="10">
         <f t="shared" si="3"/>
         <v>315</v>
       </c>
-      <c r="X16" s="11">
+      <c r="X16" s="10">
         <f>SUM($W$3:W16)+SUM(V17:$V$23)</f>
         <v>7485</v>
       </c>
-      <c r="Y16" s="11">
+      <c r="Y16" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>15</v>
-      </c>
-      <c r="B17" s="12">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11">
         <v>42499</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10">
         <v>2</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>10</v>
       </c>
-      <c r="F17" s="11">
-        <v>12</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="F17" s="10">
+        <v>12</v>
+      </c>
+      <c r="G17" s="10">
         <v>1</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>1</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <v>1</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="10">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="10">
         <v>4</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <v>4</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="10">
         <v>4</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="P17" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q17" s="11">
-        <v>15</v>
-      </c>
-      <c r="R17" s="11">
-        <v>100</v>
-      </c>
-      <c r="S17" s="11">
-        <v>100</v>
-      </c>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11">
+      <c r="P17" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>15</v>
+      </c>
+      <c r="R17" s="10">
+        <v>100</v>
+      </c>
+      <c r="S17" s="10">
+        <v>100</v>
+      </c>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W17" s="11">
+      <c r="W17" s="10">
         <f t="shared" si="3"/>
         <v>415</v>
       </c>
-      <c r="X17" s="11">
+      <c r="X17" s="10">
         <f>SUM($W$3:W17)+SUM(V18:$V$23)</f>
         <v>7520</v>
       </c>
-      <c r="Y17" s="11">
+      <c r="Y17" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>42506</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10">
         <v>2</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>10</v>
       </c>
-      <c r="F18" s="11">
-        <v>12</v>
-      </c>
-      <c r="G18" s="11">
+      <c r="F18" s="10">
+        <v>12</v>
+      </c>
+      <c r="G18" s="10">
         <v>1</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>1</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>1</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="10">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="10">
         <v>9</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="10">
         <v>5</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="10">
         <v>11</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="10">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="P18" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q18" s="11">
-        <v>15</v>
-      </c>
-      <c r="R18" s="11">
-        <v>100</v>
-      </c>
-      <c r="S18" s="11">
-        <v>100</v>
-      </c>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11">
+      <c r="P18" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>15</v>
+      </c>
+      <c r="R18" s="10">
+        <v>100</v>
+      </c>
+      <c r="S18" s="10">
+        <v>100</v>
+      </c>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W18" s="11">
+      <c r="W18" s="10">
         <f t="shared" si="3"/>
         <v>675</v>
       </c>
-      <c r="X18" s="11">
+      <c r="X18" s="10">
         <f>SUM($W$3:W18)+SUM(V19:$V$23)</f>
         <v>7815</v>
       </c>
-      <c r="Y18" s="11">
+      <c r="Y18" s="10">
         <v>8675</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="11">
         <v>42513</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <v>2</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>10</v>
       </c>
-      <c r="F19" s="11">
-        <v>12</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11">
+      <c r="F19" s="10">
+        <v>12</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K19" s="11">
-        <v>1</v>
-      </c>
-      <c r="L19" s="11">
-        <v>1</v>
-      </c>
-      <c r="M19" s="11">
-        <v>1</v>
-      </c>
-      <c r="N19" s="11">
+      <c r="K19" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="L19" s="10">
+        <v>6</v>
+      </c>
+      <c r="M19" s="10">
+        <v>8.5</v>
+      </c>
+      <c r="N19" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="O19" s="11">
+        <v>24</v>
+      </c>
+      <c r="O19" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="P19" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11">
-        <v>100</v>
-      </c>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11">
-        <v>100</v>
-      </c>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11">
+        <v>24</v>
+      </c>
+      <c r="P19" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>15</v>
+      </c>
+      <c r="R19" s="10">
+        <v>100</v>
+      </c>
+      <c r="S19" s="10">
+        <v>100</v>
+      </c>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10">
+        <f t="shared" si="2"/>
+        <v>380</v>
+      </c>
+      <c r="W19" s="10">
+        <f t="shared" si="3"/>
+        <v>595</v>
+      </c>
+      <c r="X19" s="10">
+        <f>SUM($W$3:W19)+SUM(V20:$V$23)</f>
+        <v>8030</v>
+      </c>
+      <c r="Y19" s="10">
+        <v>8675</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11">
+        <v>42520</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10">
+        <v>2</v>
+      </c>
+      <c r="E20" s="10">
+        <v>10</v>
+      </c>
+      <c r="F20" s="10">
+        <v>12</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10">
+        <v>100</v>
+      </c>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10">
+        <v>100</v>
+      </c>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10">
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="W19" s="11">
+      <c r="W20" s="10">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11">
+        <v>0</v>
+      </c>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10">
         <v>8675</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>18</v>
-      </c>
-      <c r="B20" s="12">
-        <v>42520</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="11">
+        <v>42527</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
         <v>2</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E21" s="10">
         <v>10</v>
       </c>
-      <c r="F20" s="11">
-        <v>12</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11">
+      <c r="F21" s="10">
+        <v>12</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11">
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O21" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P20" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11">
-        <v>100</v>
-      </c>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11">
+      <c r="P21" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10">
+        <v>100</v>
+      </c>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W20" s="11">
+      <c r="W21" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11">
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10">
         <v>8675</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>19</v>
-      </c>
-      <c r="B21" s="12">
-        <v>42527</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="11">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>20</v>
+      </c>
+      <c r="B22" s="14">
+        <v>42534</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15">
         <v>2</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E22" s="15">
         <v>10</v>
       </c>
-      <c r="F21" s="11">
-        <v>12</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11">
+      <c r="F22" s="15">
+        <v>12</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11">
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O22" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P21" s="11">
-        <v>15</v>
-      </c>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11">
-        <v>100</v>
-      </c>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11">
+      <c r="P22" s="15">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="16">
+        <v>100</v>
+      </c>
+      <c r="S22" s="10"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="W21" s="11">
+      <c r="W22" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11">
-        <v>8675</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>20</v>
-      </c>
-      <c r="B22" s="15">
-        <v>42534</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16">
-        <v>2</v>
-      </c>
-      <c r="E22" s="16">
-        <v>10</v>
-      </c>
-      <c r="F22" s="16">
-        <v>12</v>
-      </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="16">
-        <v>15</v>
-      </c>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="17">
-        <v>100</v>
-      </c>
-      <c r="S22" s="11"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11">
-        <f t="shared" si="2"/>
-        <v>380</v>
-      </c>
-      <c r="W22" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16">
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15">
         <v>8675</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="S23" s="9" t="s">
+      <c r="H23" s="29"/>
+      <c r="I23" s="30"/>
+      <c r="S23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T23" s="25">
+      <c r="T23" s="23">
         <v>1.5</v>
       </c>
-      <c r="U23" s="9" t="s">
+      <c r="U23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="V23" s="18">
+      <c r="V23" s="17">
         <f>40*22.5</f>
         <v>900</v>
       </c>
-      <c r="W23" s="19"/>
+      <c r="W23" s="18"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="U24" s="4" t="s">
+      <c r="I24" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="U24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V24" s="3">
+      <c r="V24" s="2">
         <f>SUM(V3,V4,V5,V6,V7,V8,V9,V10,V11,V12,V13,V14,V16,V15,V17,V18,V19,V20,V21,V22,V23)</f>
         <v>8665</v>
       </c>
-      <c r="W24" s="5">
+      <c r="W24" s="4">
         <f>SUM(W4,W3,W5,W6,W7,W8,W9,W10,W11,W12,W13,W14,W15,W17,W16,W18,W19,W20,W21,W22,W23)</f>
-        <v>5355</v>
+        <v>5890</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="23">
         <f>SUM(G3:G22)+SUM(K3:K22)</f>
-        <v>64.5</v>
-      </c>
-      <c r="H25">
+        <v>73</v>
+      </c>
+      <c r="H25" s="23">
         <f>SUM(H3:H22)+SUM(L3:L22)</f>
-        <v>52.5</v>
-      </c>
-      <c r="I25">
+        <v>57.5</v>
+      </c>
+      <c r="I25" s="23">
         <f>SUM(I3:I22)+SUM(M3:M22)</f>
-        <v>64.5</v>
-      </c>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="V25" s="20">
+      <c r="V25" s="19">
         <f>V24*T23+2.4</f>
         <v>12999.9</v>
       </c>
-      <c r="W25" s="21"/>
+      <c r="W25" s="20"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="23">
         <f>SUM($F$3:$F$22)/3</f>
         <v>80</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="23">
         <f t="shared" ref="H26:I26" si="5">SUM($F$3:$F$22)/3</f>
         <v>80</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="23">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>

</xml_diff>